<commit_message>
corrections fr -> en
</commit_message>
<xml_diff>
--- a/data/mythographie.xlsx
+++ b/data/mythographie.xlsx
@@ -5,11 +5,11 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Library/WebServer/Documents/mythographies/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegopellizzari/Documents/OBVIL/mythographie/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="mythographie_nodes.csv" sheetId="3" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7298" uniqueCount="3952">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7312" uniqueCount="3953">
   <si>
     <t>Francklin’s</t>
   </si>
@@ -12109,6 +12109,24 @@
   </si>
   <si>
     <t>Zeux′is</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>li</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri (Corps)"/>
+      </rPr>
+      <t>ttérature</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -12646,9 +12664,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G942"/>
   <sheetViews>
-    <sheetView zoomScale="191" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScale="191" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13519,8 +13537,8 @@
       <c r="D44">
         <v>-322</v>
       </c>
-      <c r="E44" s="10" t="s">
-        <v>3144</v>
+      <c r="E44" s="1" t="s">
+        <v>3952</v>
       </c>
       <c r="F44" t="s">
         <v>3112</v>
@@ -13729,7 +13747,7 @@
         <v>430</v>
       </c>
       <c r="E54" t="s">
-        <v>3144</v>
+        <v>3106</v>
       </c>
       <c r="F54" t="s">
         <v>3105</v>
@@ -24336,6 +24354,18 @@
       <c r="B636" t="s">
         <v>507</v>
       </c>
+      <c r="C636">
+        <v>-43</v>
+      </c>
+      <c r="D636">
+        <v>17</v>
+      </c>
+      <c r="E636" t="s">
+        <v>3106</v>
+      </c>
+      <c r="F636" t="s">
+        <v>3105</v>
+      </c>
     </row>
     <row r="637" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A637" t="s">
@@ -24593,7 +24623,7 @@
         <v>2923</v>
       </c>
     </row>
-    <row r="657" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="657" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A657" t="s">
         <v>3256</v>
       </c>
@@ -24607,7 +24637,7 @@
         <v>1921</v>
       </c>
     </row>
-    <row r="658" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="658" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A658" t="s">
         <v>2500</v>
       </c>
@@ -24621,7 +24651,7 @@
         <v>1912</v>
       </c>
     </row>
-    <row r="659" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="659" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A659" t="s">
         <v>277</v>
       </c>
@@ -24635,7 +24665,7 @@
         <v>3084</v>
       </c>
     </row>
-    <row r="660" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="660" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A660" t="s">
         <v>2501</v>
       </c>
@@ -24649,7 +24679,7 @@
         <v>1866</v>
       </c>
     </row>
-    <row r="661" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="661" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A661" t="s">
         <v>2502</v>
       </c>
@@ -24663,7 +24693,7 @@
         <v>1596</v>
       </c>
     </row>
-    <row r="662" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="662" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A662" t="s">
         <v>2043</v>
       </c>
@@ -24677,7 +24707,7 @@
         <v>1856</v>
       </c>
     </row>
-    <row r="663" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="663" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A663" t="s">
         <v>2924</v>
       </c>
@@ -24691,7 +24721,7 @@
         <v>3079</v>
       </c>
     </row>
-    <row r="664" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="664" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A664" t="s">
         <v>2926</v>
       </c>
@@ -24705,7 +24735,7 @@
         <v>1703</v>
       </c>
     </row>
-    <row r="665" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="665" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A665" t="s">
         <v>2503</v>
       </c>
@@ -24719,7 +24749,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="666" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="666" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A666" t="s">
         <v>2928</v>
       </c>
@@ -24733,7 +24763,7 @@
         <v>1763</v>
       </c>
     </row>
-    <row r="667" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="667" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A667" t="s">
         <v>2069</v>
       </c>
@@ -24747,7 +24777,7 @@
         <v>1687</v>
       </c>
     </row>
-    <row r="668" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="668" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A668" t="s">
         <v>2930</v>
       </c>
@@ -24761,7 +24791,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="669" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="669" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A669" t="s">
         <v>1298</v>
       </c>
@@ -24775,7 +24805,7 @@
         <v>1868</v>
       </c>
     </row>
-    <row r="670" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="670" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A670" t="s">
         <v>2504</v>
       </c>
@@ -24789,7 +24819,7 @@
         <v>3083</v>
       </c>
     </row>
-    <row r="671" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="671" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A671" t="s">
         <v>2505</v>
       </c>
@@ -24797,7 +24827,7 @@
         <v>1891</v>
       </c>
     </row>
-    <row r="672" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="672" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A672" t="s">
         <v>279</v>
       </c>
@@ -24810,8 +24840,14 @@
       <c r="D672">
         <v>-431</v>
       </c>
-    </row>
-    <row r="673" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E672" t="s">
+        <v>3107</v>
+      </c>
+      <c r="F672" t="s">
+        <v>3112</v>
+      </c>
+    </row>
+    <row r="673" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A673" t="s">
         <v>2832</v>
       </c>
@@ -24825,7 +24861,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="674" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="674" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A674" t="s">
         <v>2003</v>
       </c>
@@ -24839,7 +24875,7 @@
         <v>1749</v>
       </c>
     </row>
-    <row r="675" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="675" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A675" t="s">
         <v>2082</v>
       </c>
@@ -24853,7 +24889,7 @@
         <v>-318</v>
       </c>
     </row>
-    <row r="676" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="676" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A676" t="s">
         <v>2506</v>
       </c>
@@ -24867,7 +24903,7 @@
         <v>3081</v>
       </c>
     </row>
-    <row r="677" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="677" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A677" t="s">
         <v>2507</v>
       </c>
@@ -24881,7 +24917,7 @@
         <v>-470</v>
       </c>
     </row>
-    <row r="678" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="678" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A678" t="s">
         <v>2508</v>
       </c>
@@ -24895,7 +24931,7 @@
         <v>1733</v>
       </c>
     </row>
-    <row r="679" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="679" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A679" t="s">
         <v>3060</v>
       </c>
@@ -24909,7 +24945,7 @@
         <v>1464</v>
       </c>
     </row>
-    <row r="680" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="680" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A680" t="s">
         <v>280</v>
       </c>
@@ -24923,7 +24959,7 @@
         <v>1891</v>
       </c>
     </row>
-    <row r="681" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="681" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A681" t="s">
         <v>2509</v>
       </c>
@@ -24936,8 +24972,14 @@
       <c r="D681">
         <v>-438</v>
       </c>
-    </row>
-    <row r="682" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E681" t="s">
+        <v>3106</v>
+      </c>
+      <c r="F681" t="s">
+        <v>3112</v>
+      </c>
+    </row>
+    <row r="682" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A682" t="s">
         <v>2510</v>
       </c>
@@ -24951,7 +24993,7 @@
         <v>-590</v>
       </c>
     </row>
-    <row r="683" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="683" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A683" t="s">
         <v>2511</v>
       </c>
@@ -24965,7 +25007,7 @@
         <v>3080</v>
       </c>
     </row>
-    <row r="684" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="684" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A684" t="s">
         <v>285</v>
       </c>
@@ -24979,7 +25021,7 @@
         <v>1748</v>
       </c>
     </row>
-    <row r="685" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="685" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A685" t="s">
         <v>3030</v>
       </c>
@@ -24993,7 +25035,7 @@
         <v>-569</v>
       </c>
     </row>
-    <row r="686" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="686" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A686" t="s">
         <v>2512</v>
       </c>
@@ -25007,7 +25049,7 @@
         <v>1907</v>
       </c>
     </row>
-    <row r="687" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="687" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A687" t="s">
         <v>2513</v>
       </c>
@@ -25021,7 +25063,7 @@
         <v>-348</v>
       </c>
     </row>
-    <row r="688" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="688" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A688" t="s">
         <v>2514</v>
       </c>
@@ -25937,7 +25979,7 @@
         <v>1741</v>
       </c>
     </row>
-    <row r="753" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="753" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A753" t="s">
         <v>3263</v>
       </c>
@@ -25951,7 +25993,7 @@
         <v>1546</v>
       </c>
     </row>
-    <row r="754" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="754" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A754" t="s">
         <v>2952</v>
       </c>
@@ -25965,7 +26007,7 @@
         <v>1787</v>
       </c>
     </row>
-    <row r="755" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="755" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A755" t="s">
         <v>1372</v>
       </c>
@@ -25979,7 +26021,7 @@
         <v>1923</v>
       </c>
     </row>
-    <row r="756" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="756" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A756" t="s">
         <v>2540</v>
       </c>
@@ -25993,7 +26035,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="757" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="757" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A757" t="s">
         <v>2541</v>
       </c>
@@ -26007,7 +26049,7 @@
         <v>1626</v>
       </c>
     </row>
-    <row r="758" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="758" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A758" t="s">
         <v>2542</v>
       </c>
@@ -26015,7 +26057,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="759" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="759" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A759" t="s">
         <v>1376</v>
       </c>
@@ -26029,7 +26071,7 @@
         <v>1882</v>
       </c>
     </row>
-    <row r="760" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="760" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A760" t="s">
         <v>2994</v>
       </c>
@@ -26043,7 +26085,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="761" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="761" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A761" t="s">
         <v>2954</v>
       </c>
@@ -26057,7 +26099,7 @@
         <v>1794</v>
       </c>
     </row>
-    <row r="762" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="762" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A762" t="s">
         <v>3264</v>
       </c>
@@ -26070,8 +26112,14 @@
       <c r="D762">
         <v>1741</v>
       </c>
-    </row>
-    <row r="763" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E762" t="s">
+        <v>3106</v>
+      </c>
+      <c r="F762" t="s">
+        <v>3113</v>
+      </c>
+    </row>
+    <row r="763" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A763" t="s">
         <v>2543</v>
       </c>
@@ -26085,7 +26133,7 @@
         <v>3090</v>
       </c>
     </row>
-    <row r="764" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="764" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A764" t="s">
         <v>2544</v>
       </c>
@@ -26099,7 +26147,7 @@
         <v>1718</v>
       </c>
     </row>
-    <row r="765" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="765" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A765" t="s">
         <v>2956</v>
       </c>
@@ -26113,7 +26161,7 @@
         <v>1764</v>
       </c>
     </row>
-    <row r="766" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="766" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A766" t="s">
         <v>1380</v>
       </c>
@@ -26127,7 +26175,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="767" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="767" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A767" t="s">
         <v>1382</v>
       </c>
@@ -26141,7 +26189,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="768" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="768" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A768" t="s">
         <v>2958</v>
       </c>
@@ -27875,7 +27923,7 @@
         <v>1809</v>
       </c>
     </row>
-    <row r="897" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="897" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A897" t="s">
         <v>3006</v>
       </c>
@@ -27889,7 +27937,7 @@
         <v>1820</v>
       </c>
     </row>
-    <row r="898" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="898" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A898" t="s">
         <v>3008</v>
       </c>
@@ -27903,7 +27951,7 @@
         <v>1826</v>
       </c>
     </row>
-    <row r="899" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="899" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A899" t="s">
         <v>3035</v>
       </c>
@@ -27917,7 +27965,7 @@
         <v>1803</v>
       </c>
     </row>
-    <row r="900" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="900" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A900" t="s">
         <v>2608</v>
       </c>
@@ -27931,7 +27979,7 @@
         <v>1868</v>
       </c>
     </row>
-    <row r="901" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="901" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A901" t="s">
         <v>383</v>
       </c>
@@ -27944,8 +27992,14 @@
       <c r="D901">
         <v>-19</v>
       </c>
-    </row>
-    <row r="902" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E901" t="s">
+        <v>3106</v>
+      </c>
+      <c r="F901" t="s">
+        <v>3105</v>
+      </c>
+    </row>
+    <row r="902" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A902" t="s">
         <v>3014</v>
       </c>
@@ -27959,7 +28013,7 @@
         <v>1648</v>
       </c>
     </row>
-    <row r="903" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="903" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A903" t="s">
         <v>386</v>
       </c>
@@ -27972,8 +28026,14 @@
       <c r="D903">
         <v>1778</v>
       </c>
-    </row>
-    <row r="904" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E903" t="s">
+        <v>3106</v>
+      </c>
+      <c r="F903" t="s">
+        <v>3113</v>
+      </c>
+    </row>
+    <row r="904" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A904" t="s">
         <v>2609</v>
       </c>
@@ -27987,7 +28047,7 @@
         <v>1649</v>
       </c>
     </row>
-    <row r="905" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="905" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A905" t="s">
         <v>1861</v>
       </c>
@@ -27995,7 +28055,7 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="906" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="906" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A906" t="s">
         <v>2610</v>
       </c>
@@ -28009,7 +28069,7 @@
         <v>1875</v>
       </c>
     </row>
-    <row r="907" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="907" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A907" t="s">
         <v>2611</v>
       </c>
@@ -28023,7 +28083,7 @@
         <v>1883</v>
       </c>
     </row>
-    <row r="908" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="908" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A908" t="s">
         <v>1583</v>
       </c>
@@ -28037,7 +28097,7 @@
         <v>1687</v>
       </c>
     </row>
-    <row r="909" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="909" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A909" t="s">
         <v>2612</v>
       </c>
@@ -28051,7 +28111,7 @@
         <v>1823</v>
       </c>
     </row>
-    <row r="910" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="910" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A910" t="s">
         <v>2613</v>
       </c>
@@ -28065,7 +28125,7 @@
         <v>1895</v>
       </c>
     </row>
-    <row r="911" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="911" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A911" t="s">
         <v>390</v>
       </c>
@@ -28079,7 +28139,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="912" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="912" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A912" t="s">
         <v>1589</v>
       </c>
@@ -28311,7 +28371,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="929" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="929" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A929" t="s">
         <v>2622</v>
       </c>
@@ -28325,7 +28385,7 @@
         <v>1860</v>
       </c>
     </row>
-    <row r="930" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="930" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A930" t="s">
         <v>2623</v>
       </c>
@@ -28339,7 +28399,7 @@
         <v>1898</v>
       </c>
     </row>
-    <row r="931" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="931" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A931" t="s">
         <v>1619</v>
       </c>
@@ -28353,7 +28413,7 @@
         <v>1816</v>
       </c>
     </row>
-    <row r="932" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="932" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A932" t="s">
         <v>2624</v>
       </c>
@@ -28367,7 +28427,7 @@
         <v>1892</v>
       </c>
     </row>
-    <row r="933" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="933" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A933" t="s">
         <v>392</v>
       </c>
@@ -28381,7 +28441,7 @@
         <v>1850</v>
       </c>
     </row>
-    <row r="934" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="934" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A934" t="s">
         <v>393</v>
       </c>
@@ -28395,7 +28455,7 @@
         <v>1866</v>
       </c>
     </row>
-    <row r="935" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="935" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A935" t="s">
         <v>2625</v>
       </c>
@@ -28409,7 +28469,7 @@
         <v>1542</v>
       </c>
     </row>
-    <row r="936" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="936" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A936" t="s">
         <v>2626</v>
       </c>
@@ -28423,7 +28483,7 @@
         <v>-355</v>
       </c>
     </row>
-    <row r="937" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="937" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A937" t="s">
         <v>2232</v>
       </c>
@@ -28431,7 +28491,7 @@
         <v>2244</v>
       </c>
     </row>
-    <row r="938" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="938" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A938" t="s">
         <v>394</v>
       </c>
@@ -28444,8 +28504,14 @@
       <c r="D938">
         <v>1765</v>
       </c>
-    </row>
-    <row r="939" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E938" t="s">
+        <v>3106</v>
+      </c>
+      <c r="F938" t="s">
+        <v>3108</v>
+      </c>
+    </row>
+    <row r="939" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A939" t="s">
         <v>2627</v>
       </c>
@@ -28459,7 +28525,7 @@
         <v>3087</v>
       </c>
     </row>
-    <row r="940" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="940" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A940" t="s">
         <v>2210</v>
       </c>
@@ -28473,7 +28539,7 @@
         <v>-398</v>
       </c>
     </row>
-    <row r="941" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="941" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A941" t="s">
         <v>2628</v>
       </c>
@@ -28487,7 +28553,7 @@
         <v>1907</v>
       </c>
     </row>
-    <row r="942" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="942" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A942" t="s">
         <v>3036</v>
       </c>
@@ -42933,7 +42999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B734"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B734"/>
     </sheetView>
   </sheetViews>

</xml_diff>